<commit_message>
Implemented Tour and User controller and service except token
</commit_message>
<xml_diff>
--- a/pre-work-items/APIs_List.xlsx
+++ b/pre-work-items/APIs_List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chetan\techWork\Projects\JavaSpringAI\TeamProject\TourTravels\pre-work-items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068D1DE0-3839-4DBD-AC62-ACA1D0E5DEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0E1B4C-63AC-40CC-8478-DF9B5BA68C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{69B23AAF-014F-4780-89ED-4555FD833597}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>Feature</t>
   </si>
@@ -402,6 +402,15 @@
   </si>
   <si>
     <t>&lt;update user same as user response&gt;</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Maitri</t>
   </si>
 </sst>
 </file>
@@ -439,7 +448,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +464,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -534,16 +549,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -553,13 +564,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -570,11 +586,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1011,317 +1036,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887F652C-0617-41E3-AB72-876C27D9646A}">
-  <dimension ref="A3:G17"/>
+  <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="55.109375" customWidth="1"/>
-    <col min="7" max="7" width="42.6640625" customWidth="1"/>
+    <col min="1" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" customWidth="1"/>
+    <col min="8" max="8" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="187.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="3" t="s">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="187.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="9"/>
-      <c r="B6" s="3" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="15"/>
+      <c r="B6" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="9"/>
-      <c r="B7" s="3" t="s">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="9"/>
-      <c r="B8" s="3" t="s">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="15"/>
+      <c r="B8" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="243" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="243" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="100.8">
-      <c r="A10" s="17" t="s">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="100.8">
+      <c r="A10" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H10" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="86.4">
-      <c r="A11" s="18"/>
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:8" ht="86.4">
+      <c r="A11" s="17"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="273.60000000000002">
-      <c r="A12" s="18"/>
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="1:8" ht="273.60000000000002">
+      <c r="A12" s="17"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="F12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="172.8">
-      <c r="A13" s="19"/>
-      <c r="B13" s="6" t="s">
+    <row r="13" spans="1:8" ht="172.8">
+      <c r="A13" s="18"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="144">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:8" ht="144">
+      <c r="A14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="115.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:8" ht="115.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="115.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:8" ht="115.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.8">
-      <c r="A17" s="9"/>
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:8" ht="28.8">
+      <c r="A17" s="15"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="H17" s="14" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>